<commit_message>
heavy corvette test data (partial)
</commit_message>
<xml_diff>
--- a/TestData/hw1 multiguns.xlsx
+++ b/TestData/hw1 multiguns.xlsx
@@ -7,11 +7,10 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1 (OLD)" sheetId="1" r:id="rId1"/>
-    <sheet name="2.3 v8 commit 64" sheetId="2" r:id="rId2"/>
+    <sheet name="2.3 b7" sheetId="1" r:id="rId1"/>
+    <sheet name="2.3 b8 commit 64" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="21">
   <si>
     <t>kus</t>
   </si>
@@ -80,16 +79,10 @@
     <t>tai</t>
   </si>
   <si>
-    <t>Cloaked branch</t>
+    <t>ints</t>
   </si>
   <si>
-    <t>64 commits ahead of master</t>
-  </si>
-  <si>
-    <t>2.3 version 8</t>
-  </si>
-  <si>
-    <t>ints</t>
+    <t>2.3 build 8 Cloaked branch commit 64</t>
   </si>
 </sst>
 </file>
@@ -137,10 +130,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -556,24 +549,24 @@
       </c>
     </row>
     <row r="13" spans="2:11">
-      <c r="B13" s="1">
+      <c r="B13" s="2">
         <v>2</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="2">
         <f t="shared" ref="C13:C22" si="0">(B13 * 5)</f>
         <v>10</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="2">
         <v>2</v>
       </c>
       <c r="E13">
         <v>89.2</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13" s="2">
         <f t="shared" ref="F13:F22" si="1">AVERAGE(E13:E17)</f>
         <v>79.38000000000001</v>
       </c>
-      <c r="G13" s="1">
+      <c r="G13" s="2">
         <f t="shared" ref="G13:G22" si="2">MAX(E13:E17)-MIN(E13:E17)</f>
         <v>24.900000000000006</v>
       </c>
@@ -592,20 +585,20 @@
       </c>
     </row>
     <row r="14" spans="2:11">
-      <c r="B14" s="1"/>
-      <c r="C14" s="1">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D14" s="1"/>
+      <c r="D14" s="2"/>
       <c r="E14">
         <v>83.7</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14" s="2">
         <f t="shared" si="1"/>
         <v>81.179999999999993</v>
       </c>
-      <c r="G14" s="1">
+      <c r="G14" s="2">
         <f t="shared" si="2"/>
         <v>33.900000000000006</v>
       </c>
@@ -624,20 +617,20 @@
       </c>
     </row>
     <row r="15" spans="2:11">
-      <c r="B15" s="1"/>
-      <c r="C15" s="1">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D15" s="1"/>
+      <c r="D15" s="2"/>
       <c r="E15">
         <v>76.099999999999994</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F15" s="2">
         <f t="shared" si="1"/>
         <v>82.3</v>
       </c>
-      <c r="G15" s="1">
+      <c r="G15" s="2">
         <f t="shared" si="2"/>
         <v>33.900000000000006</v>
       </c>
@@ -656,20 +649,20 @@
       </c>
     </row>
     <row r="16" spans="2:11">
-      <c r="B16" s="1"/>
-      <c r="C16" s="1">
+      <c r="B16" s="2"/>
+      <c r="C16" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D16" s="1"/>
+      <c r="D16" s="2"/>
       <c r="E16">
         <v>83.6</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F16" s="2">
         <f t="shared" si="1"/>
         <v>87.47999999999999</v>
       </c>
-      <c r="G16" s="1">
+      <c r="G16" s="2">
         <f t="shared" si="2"/>
         <v>37.700000000000003</v>
       </c>
@@ -688,20 +681,20 @@
       </c>
     </row>
     <row r="17" spans="2:20">
-      <c r="B17" s="1"/>
-      <c r="C17" s="1">
+      <c r="B17" s="2"/>
+      <c r="C17" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D17" s="1"/>
+      <c r="D17" s="2"/>
       <c r="E17">
         <v>64.3</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F17" s="2">
         <f t="shared" si="1"/>
         <v>88.04</v>
       </c>
-      <c r="G17" s="1">
+      <c r="G17" s="2">
         <f t="shared" si="2"/>
         <v>37.700000000000003</v>
       </c>
@@ -720,24 +713,24 @@
       </c>
     </row>
     <row r="18" spans="2:20">
-      <c r="B18" s="1">
+      <c r="B18" s="2">
         <v>4</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18" s="2">
         <v>2</v>
       </c>
       <c r="E18">
         <v>98.2</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F18" s="2">
         <f t="shared" si="1"/>
         <v>101.3</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G18" s="2">
         <f t="shared" si="2"/>
         <v>44.199999999999989</v>
       </c>
@@ -756,20 +749,20 @@
       </c>
     </row>
     <row r="19" spans="2:20">
-      <c r="B19" s="1"/>
-      <c r="C19" s="1">
+      <c r="B19" s="2"/>
+      <c r="C19" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D19" s="1"/>
+      <c r="D19" s="2"/>
       <c r="E19">
         <v>89.3</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F19" s="2">
         <f t="shared" si="1"/>
         <v>102.07500000000002</v>
       </c>
-      <c r="G19" s="1">
+      <c r="G19" s="2">
         <f t="shared" si="2"/>
         <v>44.199999999999989</v>
       </c>
@@ -788,20 +781,20 @@
       </c>
     </row>
     <row r="20" spans="2:20">
-      <c r="B20" s="1"/>
-      <c r="C20" s="1">
+      <c r="B20" s="2"/>
+      <c r="C20" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D20" s="1"/>
+      <c r="D20" s="2"/>
       <c r="E20">
         <v>102</v>
       </c>
-      <c r="F20" s="1">
+      <c r="F20" s="2">
         <f t="shared" si="1"/>
         <v>106.33333333333333</v>
       </c>
-      <c r="G20" s="1">
+      <c r="G20" s="2">
         <f t="shared" si="2"/>
         <v>44.199999999999989</v>
       </c>
@@ -820,20 +813,20 @@
       </c>
     </row>
     <row r="21" spans="2:20">
-      <c r="B21" s="1"/>
-      <c r="C21" s="1">
+      <c r="B21" s="2"/>
+      <c r="C21" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D21" s="1"/>
+      <c r="D21" s="2"/>
       <c r="E21">
         <v>86.4</v>
       </c>
-      <c r="F21" s="1">
+      <c r="F21" s="2">
         <f t="shared" si="1"/>
         <v>113.66666666666667</v>
       </c>
-      <c r="G21" s="1">
+      <c r="G21" s="2">
         <f t="shared" si="2"/>
         <v>44.199999999999989</v>
       </c>
@@ -852,20 +845,20 @@
       </c>
     </row>
     <row r="22" spans="2:20">
-      <c r="B22" s="1"/>
-      <c r="C22" s="1">
+      <c r="B22" s="2"/>
+      <c r="C22" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D22" s="1"/>
+      <c r="D22" s="2"/>
       <c r="E22">
         <v>130.6</v>
       </c>
-      <c r="F22" s="1">
+      <c r="F22" s="2">
         <f t="shared" si="1"/>
         <v>120.86666666666667</v>
       </c>
-      <c r="G22" s="1">
+      <c r="G22" s="2">
         <f t="shared" si="2"/>
         <v>22.599999999999994</v>
       </c>
@@ -915,24 +908,24 @@
       </c>
     </row>
     <row r="25" spans="2:20">
-      <c r="B25" s="1">
+      <c r="B25" s="2">
         <v>4</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25" s="2">
         <f t="shared" ref="C25:C34" si="4">(B25 * 5)</f>
         <v>20</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D25" s="2">
         <v>4</v>
       </c>
       <c r="E25">
         <v>124</v>
       </c>
-      <c r="F25" s="1">
+      <c r="F25" s="2">
         <f t="shared" ref="F25:F31" si="5">AVERAGE(E25:E29)</f>
         <v>103.46</v>
       </c>
-      <c r="G25" s="1">
+      <c r="G25" s="2">
         <f t="shared" ref="G25:G31" si="6">MAX(E25:E29)-MIN(E25:E29)</f>
         <v>34.599999999999994</v>
       </c>
@@ -969,20 +962,20 @@
       </c>
     </row>
     <row r="26" spans="2:20">
-      <c r="B26" s="1"/>
-      <c r="C26" s="1">
+      <c r="B26" s="2"/>
+      <c r="C26" s="2">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="D26" s="1"/>
+      <c r="D26" s="2"/>
       <c r="E26">
         <v>108</v>
       </c>
-      <c r="F26" s="1">
+      <c r="F26" s="2">
         <f t="shared" si="5"/>
         <v>97.08</v>
       </c>
-      <c r="G26" s="1">
+      <c r="G26" s="2">
         <f t="shared" si="6"/>
         <v>18.599999999999994</v>
       </c>
@@ -1019,20 +1012,20 @@
       </c>
     </row>
     <row r="27" spans="2:20">
-      <c r="B27" s="1"/>
-      <c r="C27" s="1">
+      <c r="B27" s="2"/>
+      <c r="C27" s="2">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="D27" s="1"/>
+      <c r="D27" s="2"/>
       <c r="E27">
         <v>89.4</v>
       </c>
-      <c r="F27" s="1">
+      <c r="F27" s="2">
         <f t="shared" si="5"/>
         <v>94.039999999999992</v>
       </c>
-      <c r="G27" s="1">
+      <c r="G27" s="2">
         <f t="shared" si="6"/>
         <v>9.6999999999999886</v>
       </c>
@@ -1069,20 +1062,20 @@
       </c>
     </row>
     <row r="28" spans="2:20">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1">
+      <c r="B28" s="2"/>
+      <c r="C28" s="2">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="D28" s="1"/>
+      <c r="D28" s="2"/>
       <c r="E28">
         <v>96.8</v>
       </c>
-      <c r="F28" s="1">
+      <c r="F28" s="2">
         <f t="shared" si="5"/>
         <v>90.84</v>
       </c>
-      <c r="G28" s="1">
+      <c r="G28" s="2">
         <f t="shared" si="6"/>
         <v>25.699999999999989</v>
       </c>
@@ -1101,20 +1094,20 @@
       </c>
     </row>
     <row r="29" spans="2:20">
-      <c r="B29" s="1"/>
-      <c r="C29" s="1">
+      <c r="B29" s="2"/>
+      <c r="C29" s="2">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="D29" s="1"/>
+      <c r="D29" s="2"/>
       <c r="E29">
         <v>99.1</v>
       </c>
-      <c r="F29" s="1">
+      <c r="F29" s="2">
         <f t="shared" si="5"/>
         <v>88.179999999999993</v>
       </c>
-      <c r="G29" s="1">
+      <c r="G29" s="2">
         <f t="shared" si="6"/>
         <v>25.699999999999989</v>
       </c>
@@ -1133,24 +1126,24 @@
       </c>
     </row>
     <row r="30" spans="2:20">
-      <c r="B30" s="1">
+      <c r="B30" s="2">
         <v>8</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C30" s="2">
         <f t="shared" si="4"/>
         <v>40</v>
       </c>
-      <c r="D30" s="1">
+      <c r="D30" s="2">
         <v>4</v>
       </c>
       <c r="E30">
         <v>92.1</v>
       </c>
-      <c r="F30" s="1">
+      <c r="F30" s="2">
         <f t="shared" si="5"/>
         <v>88.919999999999987</v>
       </c>
-      <c r="G30" s="1">
+      <c r="G30" s="2">
         <f t="shared" si="6"/>
         <v>29.399999999999991</v>
       </c>
@@ -1169,20 +1162,20 @@
       </c>
     </row>
     <row r="31" spans="2:20">
-      <c r="B31" s="1"/>
-      <c r="C31" s="1">
+      <c r="B31" s="2"/>
+      <c r="C31" s="2">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="D31" s="1"/>
+      <c r="D31" s="2"/>
       <c r="E31">
         <v>92.8</v>
       </c>
-      <c r="F31" s="1">
+      <c r="F31" s="2">
         <f t="shared" si="5"/>
         <v>88.125</v>
       </c>
-      <c r="G31" s="1">
+      <c r="G31" s="2">
         <f t="shared" si="6"/>
         <v>29.399999999999991</v>
       </c>
@@ -1201,20 +1194,20 @@
       </c>
     </row>
     <row r="32" spans="2:20">
-      <c r="B32" s="1"/>
-      <c r="C32" s="1">
+      <c r="B32" s="2"/>
+      <c r="C32" s="2">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="D32" s="1"/>
+      <c r="D32" s="2"/>
       <c r="E32">
         <v>73.400000000000006</v>
       </c>
-      <c r="F32" s="1">
+      <c r="F32" s="2">
         <f>AVERAGE(E41:E45)</f>
         <v>117.34</v>
       </c>
-      <c r="G32" s="1">
+      <c r="G32" s="2">
         <f>MAX(E41:E45)-MIN(E41:E45)</f>
         <v>134.60000000000002</v>
       </c>
@@ -1233,20 +1226,20 @@
       </c>
     </row>
     <row r="33" spans="2:11">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1">
+      <c r="B33" s="2"/>
+      <c r="C33" s="2">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="D33" s="1"/>
+      <c r="D33" s="2"/>
       <c r="E33">
         <v>83.5</v>
       </c>
-      <c r="F33" s="1">
+      <c r="F33" s="2">
         <f>AVERAGE(E42:E46)</f>
         <v>108.43999999999998</v>
       </c>
-      <c r="G33" s="1">
+      <c r="G33" s="2">
         <f>MAX(E42:E46)-MIN(E42:E46)</f>
         <v>134.60000000000002</v>
       </c>
@@ -1265,20 +1258,20 @@
       </c>
     </row>
     <row r="34" spans="2:11">
-      <c r="B34" s="1"/>
-      <c r="C34" s="1">
+      <c r="B34" s="2"/>
+      <c r="C34" s="2">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="D34" s="1"/>
+      <c r="D34" s="2"/>
       <c r="E34">
         <v>102.8</v>
       </c>
-      <c r="F34" s="1">
+      <c r="F34" s="2">
         <f>AVERAGE(E43:E47)</f>
         <v>117.25000000000001</v>
       </c>
-      <c r="G34" s="1">
+      <c r="G34" s="2">
         <f>MAX(E43:E47)-MIN(E43:E47)</f>
         <v>131</v>
       </c>
@@ -1307,24 +1300,24 @@
       </c>
     </row>
     <row r="37" spans="2:11">
-      <c r="B37" s="1">
+      <c r="B37" s="2">
         <v>8</v>
       </c>
-      <c r="C37" s="1">
+      <c r="C37" s="2">
         <f t="shared" ref="C37:C46" si="8">(B37 * 5)</f>
         <v>40</v>
       </c>
-      <c r="D37" s="1">
+      <c r="D37" s="2">
         <v>8</v>
       </c>
       <c r="E37">
         <v>111.6</v>
       </c>
-      <c r="F37" s="1">
+      <c r="F37" s="2">
         <f t="shared" ref="F37:F42" si="9">AVERAGE(E37:E41)</f>
         <v>107.3</v>
       </c>
-      <c r="G37" s="1">
+      <c r="G37" s="2">
         <f t="shared" ref="G37:G42" si="10">MAX(E37:E41)-MIN(E37:E41)</f>
         <v>64.800000000000011</v>
       </c>
@@ -1343,20 +1336,20 @@
       </c>
     </row>
     <row r="38" spans="2:11">
-      <c r="B38" s="1"/>
-      <c r="C38" s="1">
+      <c r="B38" s="2"/>
+      <c r="C38" s="2">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="D38" s="1"/>
+      <c r="D38" s="2"/>
       <c r="E38">
         <v>73</v>
       </c>
-      <c r="F38" s="1">
+      <c r="F38" s="2">
         <f t="shared" si="9"/>
         <v>99.62</v>
       </c>
-      <c r="G38" s="1">
+      <c r="G38" s="2">
         <f t="shared" si="10"/>
         <v>64.800000000000011</v>
       </c>
@@ -1375,20 +1368,20 @@
       </c>
     </row>
     <row r="39" spans="2:11">
-      <c r="B39" s="1"/>
-      <c r="C39" s="1">
+      <c r="B39" s="2"/>
+      <c r="C39" s="2">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="D39" s="1"/>
+      <c r="D39" s="2"/>
       <c r="E39">
         <v>137.80000000000001</v>
       </c>
-      <c r="F39" s="1">
+      <c r="F39" s="2">
         <f t="shared" si="9"/>
         <v>126.58000000000001</v>
       </c>
-      <c r="G39" s="1">
+      <c r="G39" s="2">
         <f t="shared" si="10"/>
         <v>134.60000000000002</v>
       </c>
@@ -1407,20 +1400,20 @@
       </c>
     </row>
     <row r="40" spans="2:11">
-      <c r="B40" s="1"/>
-      <c r="C40" s="1">
+      <c r="B40" s="2"/>
+      <c r="C40" s="2">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="D40" s="1"/>
+      <c r="D40" s="2"/>
       <c r="E40">
         <v>92.8</v>
       </c>
-      <c r="F40" s="1">
+      <c r="F40" s="2">
         <f t="shared" si="9"/>
         <v>116.32000000000001</v>
       </c>
-      <c r="G40" s="1">
+      <c r="G40" s="2">
         <f t="shared" si="10"/>
         <v>134.60000000000002</v>
       </c>
@@ -1439,20 +1432,20 @@
       </c>
     </row>
     <row r="41" spans="2:11">
-      <c r="B41" s="1"/>
-      <c r="C41" s="1">
+      <c r="B41" s="2"/>
+      <c r="C41" s="2">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="D41" s="1"/>
+      <c r="D41" s="2"/>
       <c r="E41">
         <v>121.3</v>
       </c>
-      <c r="F41" s="1">
+      <c r="F41" s="2">
         <f t="shared" si="9"/>
         <v>117.34</v>
       </c>
-      <c r="G41" s="1">
+      <c r="G41" s="2">
         <f t="shared" si="10"/>
         <v>134.60000000000002</v>
       </c>
@@ -1471,24 +1464,24 @@
       </c>
     </row>
     <row r="42" spans="2:11">
-      <c r="B42" s="1">
+      <c r="B42" s="2">
         <v>16</v>
       </c>
-      <c r="C42" s="1">
+      <c r="C42" s="2">
         <f t="shared" si="8"/>
         <v>80</v>
       </c>
-      <c r="D42" s="1">
+      <c r="D42" s="2">
         <v>8</v>
       </c>
       <c r="E42">
         <v>73.2</v>
       </c>
-      <c r="F42" s="1">
+      <c r="F42" s="2">
         <f t="shared" si="9"/>
         <v>108.43999999999998</v>
       </c>
-      <c r="G42" s="1">
+      <c r="G42" s="2">
         <f t="shared" si="10"/>
         <v>134.60000000000002</v>
       </c>
@@ -1507,20 +1500,20 @@
       </c>
     </row>
     <row r="43" spans="2:11">
-      <c r="B43" s="1"/>
-      <c r="C43" s="1">
+      <c r="B43" s="2"/>
+      <c r="C43" s="2">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="D43" s="1"/>
+      <c r="D43" s="2"/>
       <c r="E43">
         <v>207.8</v>
       </c>
-      <c r="F43" s="1">
+      <c r="F43" s="2">
         <f>AVERAGE(E69:E71)</f>
         <v>124.35</v>
       </c>
-      <c r="G43" s="1">
+      <c r="G43" s="2">
         <f>MAX(E69:E71)-MIN(E69:E71)</f>
         <v>0.5</v>
       </c>
@@ -1539,20 +1532,20 @@
       </c>
     </row>
     <row r="44" spans="2:11">
-      <c r="B44" s="1"/>
-      <c r="C44" s="1">
+      <c r="B44" s="2"/>
+      <c r="C44" s="2">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="D44" s="1"/>
+      <c r="D44" s="2"/>
       <c r="E44">
         <v>86.5</v>
       </c>
-      <c r="F44" s="1">
+      <c r="F44" s="2">
         <f>AVERAGE(E70:E73)</f>
         <v>102.1</v>
       </c>
-      <c r="G44" s="1">
+      <c r="G44" s="2">
         <f>MAX(E70:E73)-MIN(E70:E73)</f>
         <v>45</v>
       </c>
@@ -1571,20 +1564,20 @@
       </c>
     </row>
     <row r="45" spans="2:11">
-      <c r="B45" s="1"/>
-      <c r="C45" s="1">
+      <c r="B45" s="2"/>
+      <c r="C45" s="2">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="D45" s="1"/>
+      <c r="D45" s="2"/>
       <c r="E45">
         <v>97.9</v>
       </c>
-      <c r="F45" s="1">
+      <c r="F45" s="2">
         <f>AVERAGE(E71:E74)</f>
         <v>82.8</v>
       </c>
-      <c r="G45" s="1">
+      <c r="G45" s="2">
         <f>MAX(E71:E74)-MIN(E71:E74)</f>
         <v>6.4000000000000057</v>
       </c>
@@ -1603,20 +1596,20 @@
       </c>
     </row>
     <row r="46" spans="2:11">
-      <c r="B46" s="1"/>
-      <c r="C46" s="1">
+      <c r="B46" s="2"/>
+      <c r="C46" s="2">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="D46" s="1"/>
+      <c r="D46" s="2"/>
       <c r="E46">
         <v>76.8</v>
       </c>
-      <c r="F46" s="1" t="e">
+      <c r="F46" s="2" t="e">
         <f>AVERAGE(#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="G46" s="1" t="e">
+      <c r="G46" s="2" t="e">
         <f>MAX(#REF!)-MIN(#REF!)</f>
         <v>#REF!</v>
       </c>
@@ -1640,24 +1633,24 @@
       </c>
     </row>
     <row r="48" spans="2:11">
-      <c r="B48" s="1">
+      <c r="B48" s="2">
         <v>16</v>
       </c>
-      <c r="C48" s="1">
+      <c r="C48" s="2">
         <f>(B48 * 5)</f>
         <v>80</v>
       </c>
-      <c r="D48" s="1">
+      <c r="D48" s="2">
         <v>16</v>
       </c>
       <c r="E48">
         <v>102.8</v>
       </c>
-      <c r="F48" s="1">
+      <c r="F48" s="2">
         <f>AVERAGE(E48:E52)</f>
         <v>111.54</v>
       </c>
-      <c r="G48" s="1">
+      <c r="G48" s="2">
         <f>MAX(E48:E52)-MIN(E48:E52)</f>
         <v>32.5</v>
       </c>
@@ -1676,20 +1669,20 @@
       </c>
     </row>
     <row r="49" spans="2:11">
-      <c r="B49" s="1"/>
-      <c r="C49" s="1">
+      <c r="B49" s="2"/>
+      <c r="C49" s="2">
         <f>(B49 * 5)</f>
         <v>0</v>
       </c>
-      <c r="D49" s="1"/>
+      <c r="D49" s="2"/>
       <c r="E49">
         <v>130.6</v>
       </c>
-      <c r="F49" s="1">
+      <c r="F49" s="2">
         <f>AVERAGE(E85:E89)</f>
         <v>98.16</v>
       </c>
-      <c r="G49" s="1">
+      <c r="G49" s="2">
         <f>MAX(E85:E89)-MIN(E85:E89)</f>
         <v>38.299999999999997</v>
       </c>
@@ -1708,20 +1701,20 @@
       </c>
     </row>
     <row r="50" spans="2:11">
-      <c r="B50" s="1"/>
-      <c r="C50" s="1">
+      <c r="B50" s="2"/>
+      <c r="C50" s="2">
         <f>(B50 * 5)</f>
         <v>0</v>
       </c>
-      <c r="D50" s="1"/>
+      <c r="D50" s="2"/>
       <c r="E50">
         <v>127.5</v>
       </c>
-      <c r="F50" s="1">
+      <c r="F50" s="2">
         <f>AVERAGE(E86:E90)</f>
         <v>97.52</v>
       </c>
-      <c r="G50" s="1">
+      <c r="G50" s="2">
         <f>MAX(E86:E90)-MIN(E86:E90)</f>
         <v>38.299999999999997</v>
       </c>
@@ -1740,20 +1733,20 @@
       </c>
     </row>
     <row r="51" spans="2:11">
-      <c r="B51" s="1"/>
-      <c r="C51" s="1">
+      <c r="B51" s="2"/>
+      <c r="C51" s="2">
         <f>(B51 * 5)</f>
         <v>0</v>
       </c>
-      <c r="D51" s="1"/>
+      <c r="D51" s="2"/>
       <c r="E51">
         <v>98.1</v>
       </c>
-      <c r="F51" s="1">
+      <c r="F51" s="2">
         <f>AVERAGE(E87:E91)</f>
         <v>100.22</v>
       </c>
-      <c r="G51" s="1">
+      <c r="G51" s="2">
         <f>MAX(E87:E91)-MIN(E87:E91)</f>
         <v>45.7</v>
       </c>
@@ -1772,20 +1765,20 @@
       </c>
     </row>
     <row r="52" spans="2:11">
-      <c r="B52" s="1"/>
-      <c r="C52" s="1">
+      <c r="B52" s="2"/>
+      <c r="C52" s="2">
         <f>(B52 * 5)</f>
         <v>0</v>
       </c>
-      <c r="D52" s="1"/>
+      <c r="D52" s="2"/>
       <c r="E52">
         <v>98.7</v>
       </c>
-      <c r="F52" s="1">
+      <c r="F52" s="2">
         <f>AVERAGE(E88:E92)</f>
         <v>99.679999999999993</v>
       </c>
-      <c r="G52" s="1">
+      <c r="G52" s="2">
         <f>MAX(E88:E92)-MIN(E88:E92)</f>
         <v>45.7</v>
       </c>
@@ -1824,7 +1817,7 @@
       <c r="F60" t="s">
         <v>5</v>
       </c>
-      <c r="G60" s="2" t="s">
+      <c r="G60" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H60" t="s">
@@ -1841,24 +1834,24 @@
       </c>
     </row>
     <row r="61" spans="2:11">
-      <c r="B61" s="1">
+      <c r="B61" s="2">
         <v>2</v>
       </c>
-      <c r="C61" s="1">
+      <c r="C61" s="2">
         <f t="shared" ref="C61:C70" si="12">(B61 * 5)</f>
         <v>10</v>
       </c>
-      <c r="D61" s="1">
+      <c r="D61" s="2">
         <v>2</v>
       </c>
       <c r="E61">
         <v>54.8</v>
       </c>
-      <c r="F61" s="1">
+      <c r="F61" s="2">
         <f t="shared" ref="F61:F67" si="13">AVERAGE(E61:E65)</f>
         <v>67.718000000000004</v>
       </c>
-      <c r="G61" s="1">
+      <c r="G61" s="2">
         <f t="shared" ref="G61:G67" si="14">MAX(E61:E65)-MIN(E61:E65)</f>
         <v>34.600000000000009</v>
       </c>
@@ -1877,20 +1870,20 @@
       </c>
     </row>
     <row r="62" spans="2:11">
-      <c r="B62" s="1"/>
-      <c r="C62" s="1">
+      <c r="B62" s="2"/>
+      <c r="C62" s="2">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="D62" s="1"/>
+      <c r="D62" s="2"/>
       <c r="E62">
         <v>89.4</v>
       </c>
-      <c r="F62" s="1">
+      <c r="F62" s="2">
         <f t="shared" si="13"/>
         <v>72.078000000000003</v>
       </c>
-      <c r="G62" s="1">
+      <c r="G62" s="2">
         <f t="shared" si="14"/>
         <v>32.030000000000008</v>
       </c>
@@ -1909,20 +1902,20 @@
       </c>
     </row>
     <row r="63" spans="2:11">
-      <c r="B63" s="1"/>
-      <c r="C63" s="1">
+      <c r="B63" s="2"/>
+      <c r="C63" s="2">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="D63" s="1"/>
+      <c r="D63" s="2"/>
       <c r="E63">
         <v>70.12</v>
       </c>
-      <c r="F63" s="1">
+      <c r="F63" s="2">
         <f t="shared" si="13"/>
         <v>74.597999999999999</v>
       </c>
-      <c r="G63" s="1">
+      <c r="G63" s="2">
         <f t="shared" si="14"/>
         <v>44.63</v>
       </c>
@@ -1941,20 +1934,20 @@
       </c>
     </row>
     <row r="64" spans="2:11">
-      <c r="B64" s="1"/>
-      <c r="C64" s="1">
+      <c r="B64" s="2"/>
+      <c r="C64" s="2">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="D64" s="1"/>
+      <c r="D64" s="2"/>
       <c r="E64">
         <v>66.900000000000006</v>
       </c>
-      <c r="F64" s="1">
+      <c r="F64" s="2">
         <f t="shared" si="13"/>
         <v>80.974000000000004</v>
       </c>
-      <c r="G64" s="1">
+      <c r="G64" s="2">
         <f t="shared" si="14"/>
         <v>44.63</v>
       </c>
@@ -1973,20 +1966,20 @@
       </c>
     </row>
     <row r="65" spans="2:11">
-      <c r="B65" s="1"/>
-      <c r="C65" s="1">
+      <c r="B65" s="2"/>
+      <c r="C65" s="2">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="D65" s="1"/>
+      <c r="D65" s="2"/>
       <c r="E65">
         <v>57.37</v>
       </c>
-      <c r="F65" s="1">
+      <c r="F65" s="2">
         <f t="shared" si="13"/>
         <v>92.414000000000016</v>
       </c>
-      <c r="G65" s="1">
+      <c r="G65" s="2">
         <f t="shared" si="14"/>
         <v>66.72999999999999</v>
       </c>
@@ -2005,24 +1998,24 @@
       </c>
     </row>
     <row r="66" spans="2:11">
-      <c r="B66" s="1">
+      <c r="B66" s="2">
         <v>4</v>
       </c>
-      <c r="C66" s="1">
+      <c r="C66" s="2">
         <f t="shared" si="12"/>
         <v>20</v>
       </c>
-      <c r="D66" s="1">
+      <c r="D66" s="2">
         <v>2</v>
       </c>
       <c r="E66">
         <v>76.599999999999994</v>
       </c>
-      <c r="F66" s="1">
+      <c r="F66" s="2">
         <f t="shared" si="13"/>
         <v>105.86000000000001</v>
       </c>
-      <c r="G66" s="1">
+      <c r="G66" s="2">
         <f t="shared" si="14"/>
         <v>48</v>
       </c>
@@ -2041,20 +2034,20 @@
       </c>
     </row>
     <row r="67" spans="2:11">
-      <c r="B67" s="1"/>
-      <c r="C67" s="1">
+      <c r="B67" s="2"/>
+      <c r="C67" s="2">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="D67" s="1"/>
+      <c r="D67" s="2"/>
       <c r="E67">
         <v>102</v>
       </c>
-      <c r="F67" s="1">
+      <c r="F67" s="2">
         <f t="shared" si="13"/>
         <v>113.17500000000001</v>
       </c>
-      <c r="G67" s="1">
+      <c r="G67" s="2">
         <f t="shared" si="14"/>
         <v>22.599999999999994</v>
       </c>
@@ -2073,20 +2066,20 @@
       </c>
     </row>
     <row r="68" spans="2:11">
-      <c r="B68" s="1"/>
-      <c r="C68" s="1">
+      <c r="B68" s="2"/>
+      <c r="C68" s="2">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="D68" s="1"/>
+      <c r="D68" s="2"/>
       <c r="E68">
         <v>102</v>
       </c>
-      <c r="F68" s="1">
+      <c r="F68" s="2">
         <f>AVERAGE(E68:E71)</f>
         <v>116.89999999999999</v>
       </c>
-      <c r="G68" s="1">
+      <c r="G68" s="2">
         <f>MAX(E68:E71)-MIN(E68:E71)</f>
         <v>22.599999999999994</v>
       </c>
@@ -2105,20 +2098,20 @@
       </c>
     </row>
     <row r="69" spans="2:11">
-      <c r="B69" s="1"/>
-      <c r="C69" s="1">
+      <c r="B69" s="2"/>
+      <c r="C69" s="2">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="D69" s="1"/>
+      <c r="D69" s="2"/>
       <c r="E69">
         <v>124.1</v>
       </c>
-      <c r="F69" s="1">
+      <c r="F69" s="2">
         <f>AVERAGE(E69:E73)</f>
         <v>109.43333333333332</v>
       </c>
-      <c r="G69" s="1">
+      <c r="G69" s="2">
         <f>MAX(E69:E73)-MIN(E69:E73)</f>
         <v>45</v>
       </c>
@@ -2137,20 +2130,20 @@
       </c>
     </row>
     <row r="70" spans="2:11">
-      <c r="B70" s="1"/>
-      <c r="C70" s="1">
+      <c r="B70" s="2"/>
+      <c r="C70" s="2">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="D70" s="1"/>
+      <c r="D70" s="2"/>
       <c r="E70">
         <v>124.6</v>
       </c>
-      <c r="F70" s="1">
+      <c r="F70" s="2">
         <f>AVERAGE(E70:E74)</f>
         <v>96.733333333333334</v>
       </c>
-      <c r="G70" s="1">
+      <c r="G70" s="2">
         <f>MAX(E70:E74)-MIN(E70:E74)</f>
         <v>45</v>
       </c>
@@ -2179,24 +2172,24 @@
       </c>
     </row>
     <row r="73" spans="2:11">
-      <c r="B73" s="1">
+      <c r="B73" s="2">
         <v>4</v>
       </c>
-      <c r="C73" s="1">
+      <c r="C73" s="2">
         <f t="shared" ref="C73:C82" si="16">(B73 * 5)</f>
         <v>20</v>
       </c>
-      <c r="D73" s="1">
+      <c r="D73" s="2">
         <v>4</v>
       </c>
       <c r="E73">
         <v>79.599999999999994</v>
       </c>
-      <c r="F73" s="1">
+      <c r="F73" s="2">
         <f t="shared" ref="F73:F79" si="17">AVERAGE(E73:E77)</f>
         <v>84.78</v>
       </c>
-      <c r="G73" s="1">
+      <c r="G73" s="2">
         <f t="shared" ref="G73:G79" si="18">MAX(E73:E77)-MIN(E73:E77)</f>
         <v>28.900000000000006</v>
       </c>
@@ -2215,20 +2208,20 @@
       </c>
     </row>
     <row r="74" spans="2:11">
-      <c r="B74" s="1"/>
-      <c r="C74" s="1">
+      <c r="B74" s="2"/>
+      <c r="C74" s="2">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="D74" s="1"/>
+      <c r="D74" s="2"/>
       <c r="E74">
         <v>86</v>
       </c>
-      <c r="F74" s="1">
+      <c r="F74" s="2">
         <f t="shared" si="17"/>
         <v>100.82000000000001</v>
       </c>
-      <c r="G74" s="1">
+      <c r="G74" s="2">
         <f t="shared" si="18"/>
         <v>86.500000000000014</v>
       </c>
@@ -2247,20 +2240,20 @@
       </c>
     </row>
     <row r="75" spans="2:11">
-      <c r="B75" s="1"/>
-      <c r="C75" s="1">
+      <c r="B75" s="2"/>
+      <c r="C75" s="2">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="D75" s="1"/>
+      <c r="D75" s="2"/>
       <c r="E75">
         <v>82.8</v>
       </c>
-      <c r="F75" s="1">
+      <c r="F75" s="2">
         <f t="shared" si="17"/>
         <v>104.64000000000001</v>
       </c>
-      <c r="G75" s="1">
+      <c r="G75" s="2">
         <f t="shared" si="18"/>
         <v>86.500000000000014</v>
       </c>
@@ -2279,20 +2272,20 @@
       </c>
     </row>
     <row r="76" spans="2:11">
-      <c r="B76" s="1"/>
-      <c r="C76" s="1">
+      <c r="B76" s="2"/>
+      <c r="C76" s="2">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="D76" s="1"/>
+      <c r="D76" s="2"/>
       <c r="E76">
         <v>73.3</v>
       </c>
-      <c r="F76" s="1">
+      <c r="F76" s="2">
         <f t="shared" si="17"/>
         <v>106.55999999999999</v>
       </c>
-      <c r="G76" s="1">
+      <c r="G76" s="2">
         <f t="shared" si="18"/>
         <v>86.500000000000014</v>
       </c>
@@ -2311,20 +2304,20 @@
       </c>
     </row>
     <row r="77" spans="2:11">
-      <c r="B77" s="1"/>
-      <c r="C77" s="1">
+      <c r="B77" s="2"/>
+      <c r="C77" s="2">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="D77" s="1"/>
+      <c r="D77" s="2"/>
       <c r="E77">
         <v>102.2</v>
       </c>
-      <c r="F77" s="1">
+      <c r="F77" s="2">
         <f t="shared" si="17"/>
         <v>112.97999999999999</v>
       </c>
-      <c r="G77" s="1">
+      <c r="G77" s="2">
         <f t="shared" si="18"/>
         <v>67.400000000000006</v>
       </c>
@@ -2343,24 +2336,24 @@
       </c>
     </row>
     <row r="78" spans="2:11">
-      <c r="B78" s="1">
+      <c r="B78" s="2">
         <v>8</v>
       </c>
-      <c r="C78" s="1">
+      <c r="C78" s="2">
         <f t="shared" si="16"/>
         <v>40</v>
       </c>
-      <c r="D78" s="1">
+      <c r="D78" s="2">
         <v>4</v>
       </c>
       <c r="E78">
         <v>159.80000000000001</v>
       </c>
-      <c r="F78" s="1">
+      <c r="F78" s="2">
         <f t="shared" si="17"/>
         <v>112.93999999999998</v>
       </c>
-      <c r="G78" s="1">
+      <c r="G78" s="2">
         <f t="shared" si="18"/>
         <v>67.400000000000006</v>
       </c>
@@ -2379,20 +2372,20 @@
       </c>
     </row>
     <row r="79" spans="2:11">
-      <c r="B79" s="1"/>
-      <c r="C79" s="1">
+      <c r="B79" s="2"/>
+      <c r="C79" s="2">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="D79" s="1"/>
+      <c r="D79" s="2"/>
       <c r="E79">
         <v>105.1</v>
       </c>
-      <c r="F79" s="1">
+      <c r="F79" s="2">
         <f t="shared" si="17"/>
         <v>101.22499999999999</v>
       </c>
-      <c r="G79" s="1">
+      <c r="G79" s="2">
         <f t="shared" si="18"/>
         <v>13</v>
       </c>
@@ -2411,20 +2404,20 @@
       </c>
     </row>
     <row r="80" spans="2:11">
-      <c r="B80" s="1"/>
-      <c r="C80" s="1">
+      <c r="B80" s="2"/>
+      <c r="C80" s="2">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="D80" s="1"/>
+      <c r="D80" s="2"/>
       <c r="E80">
         <v>92.4</v>
       </c>
-      <c r="F80" s="1">
+      <c r="F80" s="2">
         <f>AVERAGE(E89:E93)</f>
         <v>113.7</v>
       </c>
-      <c r="G80" s="1">
+      <c r="G80" s="2">
         <f>MAX(E89:E93)-MIN(E89:E93)</f>
         <v>54.100000000000009</v>
       </c>
@@ -2443,20 +2436,20 @@
       </c>
     </row>
     <row r="81" spans="2:11">
-      <c r="B81" s="1"/>
-      <c r="C81" s="1">
+      <c r="B81" s="2"/>
+      <c r="C81" s="2">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="D81" s="1"/>
+      <c r="D81" s="2"/>
       <c r="E81">
         <v>105.4</v>
       </c>
-      <c r="F81" s="1">
+      <c r="F81" s="2">
         <f>AVERAGE(E90:E94)</f>
         <v>114.88000000000002</v>
       </c>
-      <c r="G81" s="1">
+      <c r="G81" s="2">
         <f>MAX(E90:E94)-MIN(E90:E94)</f>
         <v>54.100000000000009</v>
       </c>
@@ -2475,20 +2468,20 @@
       </c>
     </row>
     <row r="82" spans="2:11">
-      <c r="B82" s="1"/>
-      <c r="C82" s="1">
+      <c r="B82" s="2"/>
+      <c r="C82" s="2">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="D82" s="1"/>
+      <c r="D82" s="2"/>
       <c r="E82">
         <v>102</v>
       </c>
-      <c r="F82" s="1">
+      <c r="F82" s="2">
         <f>AVERAGE(E91:E95)</f>
         <v>121.30000000000001</v>
       </c>
-      <c r="G82" s="1">
+      <c r="G82" s="2">
         <f>MAX(E91:E95)-MIN(E91:E95)</f>
         <v>37.700000000000017</v>
       </c>
@@ -2517,24 +2510,24 @@
       </c>
     </row>
     <row r="85" spans="2:11">
-      <c r="B85" s="1">
+      <c r="B85" s="2">
         <v>8</v>
       </c>
-      <c r="C85" s="1">
+      <c r="C85" s="2">
         <f t="shared" ref="C85:C94" si="20">(B85 * 5)</f>
         <v>40</v>
       </c>
-      <c r="D85" s="1">
+      <c r="D85" s="2">
         <v>8</v>
       </c>
       <c r="E85">
         <v>92.4</v>
       </c>
-      <c r="F85" s="1">
+      <c r="F85" s="2">
         <f t="shared" ref="F85:F90" si="21">AVERAGE(E85:E89)</f>
         <v>98.16</v>
       </c>
-      <c r="G85" s="1">
+      <c r="G85" s="2">
         <f t="shared" ref="G85:G90" si="22">MAX(E85:E89)-MIN(E85:E89)</f>
         <v>38.299999999999997</v>
       </c>
@@ -2553,20 +2546,20 @@
       </c>
     </row>
     <row r="86" spans="2:11">
-      <c r="B86" s="1"/>
-      <c r="C86" s="1">
+      <c r="B86" s="2"/>
+      <c r="C86" s="2">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
-      <c r="D86" s="1"/>
+      <c r="D86" s="2"/>
       <c r="E86">
         <v>105.4</v>
       </c>
-      <c r="F86" s="1">
+      <c r="F86" s="2">
         <f t="shared" si="21"/>
         <v>97.52</v>
       </c>
-      <c r="G86" s="1">
+      <c r="G86" s="2">
         <f t="shared" si="22"/>
         <v>38.299999999999997</v>
       </c>
@@ -2585,20 +2578,20 @@
       </c>
     </row>
     <row r="87" spans="2:11">
-      <c r="B87" s="1"/>
-      <c r="C87" s="1">
+      <c r="B87" s="2"/>
+      <c r="C87" s="2">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
-      <c r="D87" s="1"/>
+      <c r="D87" s="2"/>
       <c r="E87">
         <v>108.3</v>
       </c>
-      <c r="F87" s="1">
+      <c r="F87" s="2">
         <f t="shared" si="21"/>
         <v>100.22</v>
       </c>
-      <c r="G87" s="1">
+      <c r="G87" s="2">
         <f t="shared" si="22"/>
         <v>45.7</v>
       </c>
@@ -2617,20 +2610,20 @@
       </c>
     </row>
     <row r="88" spans="2:11">
-      <c r="B88" s="1"/>
-      <c r="C88" s="1">
+      <c r="B88" s="2"/>
+      <c r="C88" s="2">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
-      <c r="D88" s="1"/>
+      <c r="D88" s="2"/>
       <c r="E88">
         <v>73.2</v>
       </c>
-      <c r="F88" s="1">
+      <c r="F88" s="2">
         <f t="shared" si="21"/>
         <v>99.679999999999993</v>
       </c>
-      <c r="G88" s="1">
+      <c r="G88" s="2">
         <f t="shared" si="22"/>
         <v>45.7</v>
       </c>
@@ -2649,20 +2642,20 @@
       </c>
     </row>
     <row r="89" spans="2:11">
-      <c r="B89" s="1"/>
-      <c r="C89" s="1">
+      <c r="B89" s="2"/>
+      <c r="C89" s="2">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
-      <c r="D89" s="1"/>
+      <c r="D89" s="2"/>
       <c r="E89">
         <v>111.5</v>
       </c>
-      <c r="F89" s="1">
+      <c r="F89" s="2">
         <f t="shared" si="21"/>
         <v>113.7</v>
       </c>
-      <c r="G89" s="1">
+      <c r="G89" s="2">
         <f t="shared" si="22"/>
         <v>54.100000000000009</v>
       </c>
@@ -2681,24 +2674,24 @@
       </c>
     </row>
     <row r="90" spans="2:11">
-      <c r="B90" s="1">
+      <c r="B90" s="2">
         <v>16</v>
       </c>
-      <c r="C90" s="1">
+      <c r="C90" s="2">
         <f t="shared" si="20"/>
         <v>80</v>
       </c>
-      <c r="D90" s="1">
+      <c r="D90" s="2">
         <v>8</v>
       </c>
       <c r="E90">
         <v>89.2</v>
       </c>
-      <c r="F90" s="1">
+      <c r="F90" s="2">
         <f t="shared" si="21"/>
         <v>114.88000000000002</v>
       </c>
-      <c r="G90" s="1">
+      <c r="G90" s="2">
         <f t="shared" si="22"/>
         <v>54.100000000000009</v>
       </c>
@@ -2717,20 +2710,20 @@
       </c>
     </row>
     <row r="91" spans="2:11">
-      <c r="B91" s="1"/>
-      <c r="C91" s="1">
+      <c r="B91" s="2"/>
+      <c r="C91" s="2">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
-      <c r="D91" s="1"/>
+      <c r="D91" s="2"/>
       <c r="E91">
         <v>118.9</v>
       </c>
-      <c r="F91" s="1" t="e">
+      <c r="F91" s="2" t="e">
         <f>AVERAGE(E113:E117)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G91" s="1">
+      <c r="G91" s="2">
         <f>MAX(E113:E117)-MIN(E113:E117)</f>
         <v>0</v>
       </c>
@@ -2749,20 +2742,20 @@
       </c>
     </row>
     <row r="92" spans="2:11">
-      <c r="B92" s="1"/>
-      <c r="C92" s="1">
+      <c r="B92" s="2"/>
+      <c r="C92" s="2">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
-      <c r="D92" s="1"/>
+      <c r="D92" s="2"/>
       <c r="E92">
         <v>105.6</v>
       </c>
-      <c r="F92" s="1" t="e">
+      <c r="F92" s="2" t="e">
         <f>AVERAGE(E114:E118)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G92" s="1">
+      <c r="G92" s="2">
         <f>MAX(E114:E118)-MIN(E114:E118)</f>
         <v>0</v>
       </c>
@@ -2781,20 +2774,20 @@
       </c>
     </row>
     <row r="93" spans="2:11">
-      <c r="B93" s="1"/>
-      <c r="C93" s="1">
+      <c r="B93" s="2"/>
+      <c r="C93" s="2">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
-      <c r="D93" s="1"/>
+      <c r="D93" s="2"/>
       <c r="E93">
         <v>143.30000000000001</v>
       </c>
-      <c r="F93" s="1" t="e">
+      <c r="F93" s="2" t="e">
         <f>AVERAGE(E115:E119)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G93" s="1">
+      <c r="G93" s="2">
         <f>MAX(E115:E119)-MIN(E115:E119)</f>
         <v>0</v>
       </c>
@@ -2813,20 +2806,20 @@
       </c>
     </row>
     <row r="94" spans="2:11">
-      <c r="B94" s="1"/>
-      <c r="C94" s="1">
+      <c r="B94" s="2"/>
+      <c r="C94" s="2">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
-      <c r="D94" s="1"/>
+      <c r="D94" s="2"/>
       <c r="E94">
         <v>117.4</v>
       </c>
-      <c r="F94" s="1" t="e">
+      <c r="F94" s="2" t="e">
         <f>AVERAGE(E116:E120)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G94" s="1">
+      <c r="G94" s="2">
         <f>MAX(E116:E120)-MIN(E116:E120)</f>
         <v>0</v>
       </c>
@@ -2850,24 +2843,24 @@
       </c>
     </row>
     <row r="96" spans="2:11">
-      <c r="B96" s="1">
+      <c r="B96" s="2">
         <v>16</v>
       </c>
-      <c r="C96" s="1">
+      <c r="C96" s="2">
         <f>(B96 * 5)</f>
         <v>80</v>
       </c>
-      <c r="D96" s="1">
+      <c r="D96" s="2">
         <v>16</v>
       </c>
       <c r="E96">
         <v>76.5</v>
       </c>
-      <c r="F96" s="1">
+      <c r="F96" s="2">
         <f>AVERAGE(E96:E100)</f>
         <v>97.52000000000001</v>
       </c>
-      <c r="G96" s="1">
+      <c r="G96" s="2">
         <f>MAX(E96:E100)-MIN(E96:E100)</f>
         <v>51</v>
       </c>
@@ -2886,20 +2879,20 @@
       </c>
     </row>
     <row r="97" spans="2:11">
-      <c r="B97" s="1"/>
-      <c r="C97" s="1">
+      <c r="B97" s="2"/>
+      <c r="C97" s="2">
         <f>(B97 * 5)</f>
         <v>0</v>
       </c>
-      <c r="D97" s="1"/>
+      <c r="D97" s="2"/>
       <c r="E97">
         <v>89.2</v>
       </c>
-      <c r="F97" s="1" t="e">
+      <c r="F97" s="2" t="e">
         <f>AVERAGE(E133:E137)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G97" s="1">
+      <c r="G97" s="2">
         <f>MAX(E133:E137)-MIN(E133:E137)</f>
         <v>0</v>
       </c>
@@ -2918,20 +2911,20 @@
       </c>
     </row>
     <row r="98" spans="2:11">
-      <c r="B98" s="1"/>
-      <c r="C98" s="1">
+      <c r="B98" s="2"/>
+      <c r="C98" s="2">
         <f>(B98 * 5)</f>
         <v>0</v>
       </c>
-      <c r="D98" s="1"/>
+      <c r="D98" s="2"/>
       <c r="E98">
         <v>92.4</v>
       </c>
-      <c r="F98" s="1" t="e">
+      <c r="F98" s="2" t="e">
         <f>AVERAGE(E134:E138)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G98" s="1">
+      <c r="G98" s="2">
         <f>MAX(E134:E138)-MIN(E134:E138)</f>
         <v>0</v>
       </c>
@@ -2950,20 +2943,20 @@
       </c>
     </row>
     <row r="99" spans="2:11">
-      <c r="B99" s="1"/>
-      <c r="C99" s="1">
+      <c r="B99" s="2"/>
+      <c r="C99" s="2">
         <f>(B99 * 5)</f>
         <v>0</v>
       </c>
-      <c r="D99" s="1"/>
+      <c r="D99" s="2"/>
       <c r="E99">
         <v>127.5</v>
       </c>
-      <c r="F99" s="1" t="e">
+      <c r="F99" s="2" t="e">
         <f>AVERAGE(E135:E139)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G99" s="1">
+      <c r="G99" s="2">
         <f>MAX(E135:E139)-MIN(E135:E139)</f>
         <v>0</v>
       </c>
@@ -2982,20 +2975,20 @@
       </c>
     </row>
     <row r="100" spans="2:11">
-      <c r="B100" s="1"/>
-      <c r="C100" s="1">
+      <c r="B100" s="2"/>
+      <c r="C100" s="2">
         <f>(B100 * 5)</f>
         <v>0</v>
       </c>
-      <c r="D100" s="1"/>
+      <c r="D100" s="2"/>
       <c r="E100">
         <v>102</v>
       </c>
-      <c r="F100" s="1" t="e">
+      <c r="F100" s="2" t="e">
         <f>AVERAGE(E136:E140)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G100" s="1">
+      <c r="G100" s="2">
         <f>MAX(E136:E140)-MIN(E136:E140)</f>
         <v>0</v>
       </c>
@@ -3220,19 +3213,13 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.42578125" defaultRowHeight="12.75"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3378,7 +3365,7 @@
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>